<commit_message>
Update ads dashboard archetypes and data integrations
</commit_message>
<xml_diff>
--- a/data/key_advantages/key_advantages.xlsx
+++ b/data/key_advantages/key_advantages.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29328"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thoma\Documents\Projects\Client event\Dashboard\data\key_advantages\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1225984-7391-4F3E-9543-41A144B86FBF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PUMA" sheetId="1" r:id="rId1"/>
@@ -12,12 +18,12 @@
     <sheet name="adidas" sheetId="3" r:id="rId3"/>
     <sheet name="Summary" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="56">
   <si>
     <t>advantage_id</t>
   </si>
@@ -96,70 +102,18 @@
     <t>More cuteness is here. Shop PUMA x Hello Kitty and Friends. (English: More cuteness is here. Shop PUMA x Hello Kitty and Friends.)</t>
   </si>
   <si>
-    <t>Up to 60% off 3–11 Nov</t>
-  </si>
-  <si>
-    <t>Extra 15% with code LEVELUP on 2+ items</t>
-  </si>
-  <si>
-    <t>Multilingual regional promo versions</t>
-  </si>
-  <si>
-    <t>Limited-time discounts</t>
-  </si>
-  <si>
-    <t>Basket-building incentive</t>
-  </si>
-  <si>
-    <t>Localized communication</t>
-  </si>
-  <si>
-    <t>Most ads push a dated promo window (03–11 Nov) with up to 60% off. | Clear deadline-driven message encourages immediate purchase.</t>
-  </si>
-  <si>
-    <t>The promo becomes stronger if the shopper buys at least two items. | The code LEVELUP is explicitly mentioned, nudging higher basket value.</t>
-  </si>
-  <si>
-    <t>The same offer is rendered in Chinese to reach local/expat audiences. | This shows the brand tailors promo messaging per market while keeping the core offer.</t>
-  </si>
-  <si>
-    <t>From 03 - 11 Nov, score up to 60% off select styles. Unlock an extra 15% off when you shop min. 2 items* with code LEVELUP (English: From 03 - 11 Nov, score up to 60% off select styles. Unlock an extra 15% off when you shop min. 2 items* with code LEVELUP)</t>
-  </si>
-  <si>
-    <t>11 月 3-11 日，精選款式最低 6 折。選購 2 件商品*以上，輸入優惠碼 LEVELUP 再享 9 折 (English: From 3–11 Nov, selected styles up to 40% off. Buy 2+ items and use code LEVELUP for extra 10%.)</t>
-  </si>
-  <si>
-    <t>Extra 35% with promo code</t>
-  </si>
-  <si>
     <t>Iconic adidas style</t>
   </si>
   <si>
-    <t>Stacked/conditional discounts</t>
-  </si>
-  <si>
     <t>Brand/style positioning</t>
   </si>
   <si>
-    <t>Multiple creatives push an extra 35% off when a code is used on full-price and sale items. | This communicates a deeper discount than the headline promo.</t>
-  </si>
-  <si>
     <t>Several ads focus on taking your style up a notch with unmistakable adidas looks in different languages. | This stresses recognisable brand-led styling over price.</t>
   </si>
   <si>
-    <t>Get an extra 35% off with code FALL on full price and sale styles. Exclusions apply.</t>
-  </si>
-  <si>
     <t>Take it up a notch in unmistakable adidas style</t>
   </si>
   <si>
-    <t>Istakni se u nepogrešivom adidas stilu</t>
-  </si>
-  <si>
-    <t>"Seçili ürünlerde %35'e varan indirime ek sepette %15 indirim başladı
-Tüm indirimlere ek sepette %15 indirim seni bekliyor."</t>
-  </si>
-  <si>
     <t>Summary</t>
   </si>
   <si>
@@ -170,13 +124,82 @@
   </si>
   <si>
     <t>adidas – Extra 35% with promo code; Iconic adidas style</t>
+  </si>
+  <si>
+    <t>Nike as a brand of personal growth</t>
+  </si>
+  <si>
+    <t>Brand empowerment</t>
+  </si>
+  <si>
+    <t>Nike continues to position itself as more than a product brand, emphasizing personal growth, individual choices, and empowerment. | This resonates strongly with consumers who value authenticity and personal journeys.</t>
+  </si>
+  <si>
+    <t>Nike allowed me to retrace my growth over the past 10 years. Where I am and who I am today are the result of choices — and of never accepting compromises. I’m an artisan, not an influencer. #nikeshox #teamnike #ad</t>
+  </si>
+  <si>
+    <t>Revolutionary product design</t>
+  </si>
+  <si>
+    <t>Innovation</t>
+  </si>
+  <si>
+    <t>Nike's focus on revolutionary technology and cutting-edge product design continues to resonate. | Ads emphasize how their products go beyond style to offer complete experiences.</t>
+  </si>
+  <si>
+    <t>DNA rivoluzionario. Esperienza totale.</t>
+  </si>
+  <si>
+    <t>It’s not just about style. It’s the energy you carry when you put them on. #nikeshox #teamnike #ad</t>
+  </si>
+  <si>
+    <t>Nike Shox as a statement product</t>
+  </si>
+  <si>
+    <t>Statement product</t>
+  </si>
+  <si>
+    <t>Nike Shox is continuously pushed as a signature product with distinct branding, showcasing its power and innovation. | This taps into the desire for high-impact, noticeable products.</t>
+  </si>
+  <si>
+    <t>Née pour déranger. L’expérience totale. (Born to disturb. The total experience.)</t>
+  </si>
+  <si>
+    <t>La nouvelle Nike Shok Z, la paire qui ne te laisse pas indifférent ✨@nike #NikeShox #TeamNike Publicité 🎥 : @mehdiscovers (The new Nike Shok Z, the pair that doesn’t leave you indifferent ✨@nike #NikeShox #TeamNike Advertisement 🎥 : @mehdiscovers)</t>
+  </si>
+  <si>
+    <t>Schalt mit unverwechselbaren adidas Styles einen Gang höher (Switch up your style with unmistakable adidas styles)</t>
+  </si>
+  <si>
+    <t>Black Friday / adiClub Sign-up Incentives</t>
+  </si>
+  <si>
+    <t>Several ads offer an incentive to sign up for adiClub to participate in exclusive offers like winning a gift card. | This creates urgency around registration and exclusivity.</t>
+  </si>
+  <si>
+    <t>In occasione del Black Friday, iscriviti ad adiClub e crea la tua wishlist per avere la possibilità di vincere una Gift Card da 250 €. (On the occasion of Black Friday, sign up for adiClub and create your wishlist for a chance to win a €250 Gift Card.)</t>
+  </si>
+  <si>
+    <t>Suscríbete a adiClub y crea tu lista de deseos para poder ganar una tarjeta regalo por valor de 250€ este Black Friday. (Sign up for adiClub and create your wishlist to win a €250 gift card this Black Friday.)</t>
+  </si>
+  <si>
+    <t>adidas Vibes Fragrance</t>
+  </si>
+  <si>
+    <t>Category extension</t>
+  </si>
+  <si>
+    <t>This ad highlights adidas's entry into the fragrance market, positioning it as part of the lifestyle beyond just apparel. | This suggests adidas is becoming synonymous with an all-around lifestyle brand.</t>
+  </si>
+  <si>
+    <t>adidas Vibes Body &amp; Hair Mist mein Frische-Boost für jeden Mood, ob vor dem Training oder beim Entspannen zuhause #adidasfragrance #createdwithadidas (adidas Vibes Body &amp; Hair Mist, my freshness boost for any mood, whether before training or relaxing at home #adidasfragrance #createdwithadidas)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -239,13 +262,21 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -283,7 +314,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -317,6 +348,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -351,9 +383,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -526,14 +559,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -553,7 +586,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -573,7 +606,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1</v>
       </c>
@@ -593,7 +626,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>2</v>
       </c>
@@ -613,7 +646,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>2</v>
       </c>
@@ -633,7 +666,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>3</v>
       </c>
@@ -653,7 +686,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>3</v>
       </c>
@@ -673,7 +706,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>4</v>
       </c>
@@ -693,7 +726,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>4</v>
       </c>
@@ -719,14 +752,16 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -746,124 +781,89 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>25</v>
+        <v>33</v>
       </c>
       <c r="C2" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="D2" t="s">
-        <v>31</v>
-      </c>
-      <c r="E2">
-        <v>1</v>
+        <v>35</v>
       </c>
       <c r="F2" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>25</v>
+        <v>37</v>
       </c>
       <c r="C3" t="s">
-        <v>28</v>
+        <v>38</v>
       </c>
       <c r="D3" t="s">
-        <v>31</v>
-      </c>
-      <c r="E3">
-        <v>14</v>
+        <v>39</v>
       </c>
       <c r="F3" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>26</v>
+        <v>37</v>
       </c>
       <c r="C4" t="s">
-        <v>29</v>
+        <v>38</v>
       </c>
       <c r="D4" t="s">
-        <v>32</v>
-      </c>
-      <c r="E4">
-        <v>1</v>
+        <v>39</v>
       </c>
       <c r="F4" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>26</v>
+        <v>42</v>
       </c>
       <c r="C5" t="s">
-        <v>29</v>
+        <v>43</v>
       </c>
       <c r="D5" t="s">
-        <v>32</v>
-      </c>
-      <c r="E5">
-        <v>14</v>
+        <v>44</v>
       </c>
       <c r="F5" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>3</v>
       </c>
       <c r="B6" t="s">
-        <v>27</v>
+        <v>42</v>
       </c>
       <c r="C6" t="s">
-        <v>30</v>
+        <v>43</v>
       </c>
       <c r="D6" t="s">
-        <v>33</v>
-      </c>
-      <c r="E6">
-        <v>29</v>
+        <v>44</v>
       </c>
       <c r="F6" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6">
-      <c r="A7">
-        <v>3</v>
-      </c>
-      <c r="B7" t="s">
-        <v>27</v>
-      </c>
-      <c r="C7" t="s">
-        <v>30</v>
-      </c>
-      <c r="D7" t="s">
-        <v>33</v>
-      </c>
-      <c r="E7">
-        <v>55</v>
-      </c>
-      <c r="F7" t="s">
-        <v>35</v>
+        <v>46</v>
       </c>
     </row>
   </sheetData>
@@ -872,14 +872,16 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I12" sqref="I12"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -899,72 +901,89 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>36</v>
+        <v>25</v>
       </c>
       <c r="C2" t="s">
-        <v>38</v>
+        <v>26</v>
       </c>
       <c r="D2" t="s">
-        <v>40</v>
+        <v>27</v>
       </c>
       <c r="F2" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>37</v>
+        <v>25</v>
       </c>
       <c r="C3" t="s">
-        <v>39</v>
+        <v>26</v>
       </c>
       <c r="D3" t="s">
-        <v>41</v>
+        <v>27</v>
       </c>
       <c r="F3" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>37</v>
+        <v>48</v>
       </c>
       <c r="C4" t="s">
-        <v>39</v>
+        <v>12</v>
       </c>
       <c r="D4" t="s">
-        <v>41</v>
+        <v>49</v>
       </c>
       <c r="F4" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>2</v>
       </c>
       <c r="B5" t="s">
-        <v>37</v>
+        <v>48</v>
       </c>
       <c r="C5" t="s">
-        <v>39</v>
+        <v>12</v>
       </c>
       <c r="D5" t="s">
-        <v>41</v>
+        <v>49</v>
       </c>
       <c r="F5" t="s">
-        <v>45</v>
+        <v>51</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>3</v>
+      </c>
+      <c r="B6" t="s">
+        <v>52</v>
+      </c>
+      <c r="C6" t="s">
+        <v>53</v>
+      </c>
+      <c r="D6" t="s">
+        <v>54</v>
+      </c>
+      <c r="F6" t="s">
+        <v>55</v>
       </c>
     </row>
   </sheetData>
@@ -973,31 +992,31 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:A4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>49</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>